<commit_message>
Edited scripts, environmental settings, added metadata, renamed notebooks, added Step1_GDB
</commit_message>
<xml_diff>
--- a/src/Domain Tables 20230414.xlsx
+++ b/src/Domain Tables 20230414.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sageg\source\repos\mas-python\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EB8D64-6B8E-4207-824F-940B3A02DE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9D3890-9DB1-4B67-91B8-0A2AF53E971C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="816" activeTab="10" xr2:uid="{74A246E4-10EC-4818-A688-D902679151D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="816" firstSheet="6" activeTab="14" xr2:uid="{74A246E4-10EC-4818-A688-D902679151D2}"/>
   </bookViews>
   <sheets>
     <sheet name="D_OBJECTIVE" sheetId="3" r:id="rId1"/>
@@ -3119,7 +3119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B787F1A-A321-4D97-8042-6A91D7475904}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
@@ -3531,7 +3531,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,7 +3634,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="19" t="s">
         <v>609</v>
@@ -3656,9 +3656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD38850E-E84E-47FF-B087-6AD4F1BF0778}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>